<commit_message>
Updated CT casade for 2017 ASR
</commit_message>
<xml_diff>
--- a/Chlamydia/data/CT notifications_2016_National_Estimate.xlsx
+++ b/Chlamydia/data/CT notifications_2016_National_Estimate.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="23955" windowHeight="12840" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="23955" windowHeight="12840"/>
   </bookViews>
   <sheets>
     <sheet name="CT notifications_2007-2016" sheetId="1" r:id="rId1"/>
@@ -674,7 +674,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -693,6 +693,8 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="35" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="35" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -711,8 +713,7 @@
     <xf numFmtId="0" fontId="0" fillId="35" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="35" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="35" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3743,8 +3744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O72"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="H71" sqref="H71:H72"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3760,23 +3761,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="20"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="22"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -4218,23 +4219,23 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="19"/>
-      <c r="M12" s="19"/>
-      <c r="N12" s="19"/>
-      <c r="O12" s="20"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="21"/>
+      <c r="M12" s="21"/>
+      <c r="N12" s="21"/>
+      <c r="O12" s="22"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -4675,24 +4676,28 @@
         <v>49285</v>
       </c>
     </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H22" s="26"/>
+      <c r="O22" s="17"/>
+    </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="18" t="s">
+      <c r="A24" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="19"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="19"/>
-      <c r="I24" s="19"/>
-      <c r="J24" s="19"/>
-      <c r="K24" s="19"/>
-      <c r="L24" s="19"/>
-      <c r="M24" s="19"/>
-      <c r="N24" s="19"/>
-      <c r="O24" s="20"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="21"/>
+      <c r="K24" s="21"/>
+      <c r="L24" s="21"/>
+      <c r="M24" s="21"/>
+      <c r="N24" s="21"/>
+      <c r="O24" s="22"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
@@ -4840,23 +4845,23 @@
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="21" t="s">
+      <c r="A30" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="22"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="22"/>
-      <c r="G30" s="22"/>
-      <c r="H30" s="22"/>
-      <c r="I30" s="22"/>
-      <c r="J30" s="22"/>
-      <c r="K30" s="22"/>
-      <c r="L30" s="22"/>
-      <c r="M30" s="22"/>
-      <c r="N30" s="22"/>
-      <c r="O30" s="23"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="24"/>
+      <c r="J30" s="24"/>
+      <c r="K30" s="24"/>
+      <c r="L30" s="24"/>
+      <c r="M30" s="24"/>
+      <c r="N30" s="24"/>
+      <c r="O30" s="25"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
@@ -5458,81 +5463,81 @@
       <c r="A41" s="9">
         <v>2016</v>
       </c>
-      <c r="B41" s="24">
+      <c r="B41" s="18">
         <f>-0.0088*10 + 0.228</f>
         <v>0.14000000000000001</v>
       </c>
-      <c r="C41" s="24">
+      <c r="C41" s="18">
         <f>0.0077*10+0.145</f>
         <v>0.22199999999999998</v>
       </c>
-      <c r="D41" s="24">
+      <c r="D41" s="18">
         <f>0.0053*10+0.2076</f>
         <v>0.2606</v>
       </c>
-      <c r="E41" s="24">
+      <c r="E41" s="18">
         <f>0.0033*10+0.2239</f>
         <v>0.25690000000000002</v>
       </c>
-      <c r="F41" s="24">
+      <c r="F41" s="18">
         <f>0.0028*10+0.2315</f>
         <v>0.25950000000000001</v>
       </c>
-      <c r="G41" s="24">
+      <c r="G41" s="18">
         <f>-0.0038*10+0.2476</f>
         <v>0.20959999999999998</v>
       </c>
-      <c r="H41" s="24">
+      <c r="H41" s="18">
         <f>0.0041*10+0.2124</f>
         <v>0.25340000000000001</v>
       </c>
-      <c r="I41" s="24">
+      <c r="I41" s="18">
         <f>0.0035*10+0.1189</f>
         <v>0.15390000000000001</v>
       </c>
-      <c r="J41" s="24">
+      <c r="J41" s="18">
         <f>0.0054*10+0.1676</f>
         <v>0.22160000000000002</v>
       </c>
-      <c r="K41" s="24">
+      <c r="K41" s="18">
         <f>0.0032*10+0.226</f>
         <v>0.25800000000000001</v>
       </c>
-      <c r="L41" s="24">
+      <c r="L41" s="18">
         <f>0.0028*10+0.2273</f>
         <v>0.25530000000000003</v>
       </c>
-      <c r="M41" s="24">
+      <c r="M41" s="18">
         <f>-0.0011*10+0.2298</f>
         <v>0.21879999999999999</v>
       </c>
-      <c r="N41" s="24">
+      <c r="N41" s="18">
         <f>-0.0023*10+0.2341</f>
         <v>0.21110000000000001</v>
       </c>
-      <c r="O41" s="25">
+      <c r="O41" s="19">
         <f>0.0038*10+0.206</f>
         <v>0.24399999999999999</v>
       </c>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A69" s="18" t="s">
+      <c r="A69" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B69" s="19"/>
-      <c r="C69" s="19"/>
-      <c r="D69" s="19"/>
-      <c r="E69" s="19"/>
-      <c r="F69" s="19"/>
-      <c r="G69" s="19"/>
-      <c r="H69" s="19"/>
-      <c r="I69" s="19"/>
-      <c r="J69" s="19"/>
-      <c r="K69" s="19"/>
-      <c r="L69" s="19"/>
-      <c r="M69" s="19"/>
-      <c r="N69" s="19"/>
-      <c r="O69" s="20"/>
+      <c r="B69" s="21"/>
+      <c r="C69" s="21"/>
+      <c r="D69" s="21"/>
+      <c r="E69" s="21"/>
+      <c r="F69" s="21"/>
+      <c r="G69" s="21"/>
+      <c r="H69" s="21"/>
+      <c r="I69" s="21"/>
+      <c r="J69" s="21"/>
+      <c r="K69" s="21"/>
+      <c r="L69" s="21"/>
+      <c r="M69" s="21"/>
+      <c r="N69" s="21"/>
+      <c r="O69" s="22"/>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
@@ -5721,7 +5726,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
@@ -5736,18 +5741,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="20"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="22"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -6054,18 +6059,18 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="20"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="22"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -6372,12 +6377,12 @@
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="18" t="s">
+      <c r="A23" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="19"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="20"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="22"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">

</xml_diff>

<commit_message>
Updated code and data for 2016 estimates
</commit_message>
<xml_diff>
--- a/Chlamydia/data/CT notifications_2016_National_Estimate.xlsx
+++ b/Chlamydia/data/CT notifications_2016_National_Estimate.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="23955" windowHeight="12840"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="23955" windowHeight="12840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CT notifications_2007-2016" sheetId="1" r:id="rId1"/>
@@ -97,7 +97,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -674,7 +674,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -695,6 +695,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="35" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="35" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -713,7 +715,6 @@
     <xf numFmtId="0" fontId="0" fillId="35" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3741,11 +3742,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O72"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q23" sqref="Q23"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="I75" sqref="I75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3761,23 +3762,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="22"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="24"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -4219,23 +4220,23 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="21"/>
-      <c r="K12" s="21"/>
-      <c r="L12" s="21"/>
-      <c r="M12" s="21"/>
-      <c r="N12" s="21"/>
-      <c r="O12" s="22"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="23"/>
+      <c r="N12" s="23"/>
+      <c r="O12" s="24"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -4677,27 +4678,27 @@
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="H22" s="26"/>
+      <c r="H22" s="20"/>
       <c r="O22" s="17"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="20" t="s">
+      <c r="A24" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="21"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="21"/>
-      <c r="H24" s="21"/>
-      <c r="I24" s="21"/>
-      <c r="J24" s="21"/>
-      <c r="K24" s="21"/>
-      <c r="L24" s="21"/>
-      <c r="M24" s="21"/>
-      <c r="N24" s="21"/>
-      <c r="O24" s="22"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="23"/>
+      <c r="I24" s="23"/>
+      <c r="J24" s="23"/>
+      <c r="K24" s="23"/>
+      <c r="L24" s="23"/>
+      <c r="M24" s="23"/>
+      <c r="N24" s="23"/>
+      <c r="O24" s="24"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
@@ -4845,23 +4846,23 @@
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="23" t="s">
+      <c r="A30" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="24"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="24"/>
-      <c r="G30" s="24"/>
-      <c r="H30" s="24"/>
-      <c r="I30" s="24"/>
-      <c r="J30" s="24"/>
-      <c r="K30" s="24"/>
-      <c r="L30" s="24"/>
-      <c r="M30" s="24"/>
-      <c r="N30" s="24"/>
-      <c r="O30" s="25"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="26"/>
+      <c r="K30" s="26"/>
+      <c r="L30" s="26"/>
+      <c r="M30" s="26"/>
+      <c r="N30" s="26"/>
+      <c r="O30" s="27"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
@@ -5521,23 +5522,23 @@
       </c>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A69" s="20" t="s">
+      <c r="A69" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B69" s="21"/>
-      <c r="C69" s="21"/>
-      <c r="D69" s="21"/>
-      <c r="E69" s="21"/>
-      <c r="F69" s="21"/>
-      <c r="G69" s="21"/>
-      <c r="H69" s="21"/>
-      <c r="I69" s="21"/>
-      <c r="J69" s="21"/>
-      <c r="K69" s="21"/>
-      <c r="L69" s="21"/>
-      <c r="M69" s="21"/>
-      <c r="N69" s="21"/>
-      <c r="O69" s="22"/>
+      <c r="B69" s="23"/>
+      <c r="C69" s="23"/>
+      <c r="D69" s="23"/>
+      <c r="E69" s="23"/>
+      <c r="F69" s="23"/>
+      <c r="G69" s="23"/>
+      <c r="H69" s="23"/>
+      <c r="I69" s="23"/>
+      <c r="J69" s="23"/>
+      <c r="K69" s="23"/>
+      <c r="L69" s="23"/>
+      <c r="M69" s="23"/>
+      <c r="N69" s="23"/>
+      <c r="O69" s="24"/>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
@@ -5707,6 +5708,19 @@
         <f t="shared" si="15"/>
         <v>53189.153439153437</v>
       </c>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J75" s="21"/>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C76" s="21"/>
+      <c r="J76" s="21"/>
+    </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C78" s="21"/>
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C79" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -5723,11 +5737,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5741,18 +5755,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="22"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="24"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -6059,18 +6073,18 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="22"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="24"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -6377,12 +6391,12 @@
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="20" t="s">
+      <c r="A23" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="21"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="22"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="24"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">

</xml_diff>